<commit_message>
update analysis paper sudoe
</commit_message>
<xml_diff>
--- a/data/Datos_boxplot_metodos.xlsx
+++ b/data/Datos_boxplot_metodos.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajpelu/Nextcloud/alcontar/veg_alcontar/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E2A7CFD-290C-3240-9F92-04D4AA3A51BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8F31375-81C1-704B-AA57-D979FB83A25C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-3140" windowWidth="38400" windowHeight="21140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16380" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fitovolumen_quadrat" sheetId="4" r:id="rId1"/>
     <sheet name="cobertura_quadrat" sheetId="3" r:id="rId2"/>
     <sheet name="cobertura_transectos" sheetId="1" r:id="rId3"/>
     <sheet name="fitovolumen_transectos" sheetId="2" r:id="rId4"/>
+    <sheet name="riqueza_div_quadrat" sheetId="5" r:id="rId5"/>
+    <sheet name="riqueza_transectos" sheetId="6" r:id="rId6"/>
+    <sheet name="diversidad_transectos" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="143">
   <si>
     <t>ZONA</t>
   </si>
@@ -430,13 +433,40 @@
   </si>
   <si>
     <t>PLOT</t>
+  </si>
+  <si>
+    <t>Nombre_zona</t>
+  </si>
+  <si>
+    <t>GEO_PARCELA.NOMBRE</t>
+  </si>
+  <si>
+    <t>GEO_QUADRAT.NOMBRE</t>
+  </si>
+  <si>
+    <t>Quadrat_riqueza</t>
+  </si>
+  <si>
+    <t>Quadrat_diversidad</t>
+  </si>
+  <si>
+    <t>Line_intercept</t>
+  </si>
+  <si>
+    <t>Point_quadrat</t>
+  </si>
+  <si>
+    <t>Point_quadrat_extenso</t>
+  </si>
+  <si>
+    <t>Quadrat_parcela</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -448,11 +478,13 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -465,6 +497,13 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -487,7 +526,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -744,14 +783,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC0C0C0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC0C0C0"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC0C0C0"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC0C0C0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFC0C0C0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -888,12 +957,44 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Cobertura" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Normal_Diversidad" xfId="4" xr:uid="{27C32369-96BF-9F44-91E6-B0652A023E5C}"/>
     <cellStyle name="Normal_Fitovolumen" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Normal_Hoja1" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal_Riqueza" xfId="5" xr:uid="{A09F8609-F9C0-5C4F-AF79-C4E3D8F58DF1}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3128,7 +3229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF374CB8-5C5E-F04B-B0DC-35589760720E}">
   <dimension ref="A1:F97"/>
   <sheetViews>
-    <sheetView topLeftCell="A83" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
@@ -5192,7 +5293,7 @@
         <v>22.918560000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>42</v>
       </c>
@@ -5212,7 +5313,7 @@
         <v>20.809439999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>42</v>
       </c>
@@ -5232,7 +5333,7 @@
         <v>14.288959999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>42</v>
       </c>
@@ -5252,7 +5353,7 @@
         <v>17.025919999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>42</v>
       </c>
@@ -5361,7 +5462,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
@@ -5633,4 +5734,2190 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17DB8484-EF1D-244D-8B3B-AC26797600F3}">
+  <dimension ref="A1:E97"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="46" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>137</v>
+      </c>
+      <c r="E1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="47" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="48">
+        <v>11</v>
+      </c>
+      <c r="E2" s="49">
+        <v>-1.6891936000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="48">
+        <v>7</v>
+      </c>
+      <c r="E3" s="50">
+        <v>-1.3672145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="47" t="s">
+        <v>36</v>
+      </c>
+      <c r="D4" s="48">
+        <v>10</v>
+      </c>
+      <c r="E4" s="50">
+        <v>-1.3019304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" s="47" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="48">
+        <v>4</v>
+      </c>
+      <c r="E5" s="50">
+        <v>-1.0213603</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="47" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="48">
+        <v>5</v>
+      </c>
+      <c r="E6" s="50">
+        <v>-1.1625105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="47" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="48">
+        <v>5</v>
+      </c>
+      <c r="E7" s="50">
+        <v>-0.42926560000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="47" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="48">
+        <v>8</v>
+      </c>
+      <c r="E8" s="50">
+        <v>-0.69446379999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="47" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="48">
+        <v>10</v>
+      </c>
+      <c r="E9" s="50">
+        <v>-1.6574287000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="48">
+        <v>10</v>
+      </c>
+      <c r="E10" s="50">
+        <v>-1.5678147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="47" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="48">
+        <v>10</v>
+      </c>
+      <c r="E11" s="50">
+        <v>-1.9490227</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="47" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="48">
+        <v>9</v>
+      </c>
+      <c r="E12" s="50">
+        <v>-1.4902842999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="48">
+        <v>11</v>
+      </c>
+      <c r="E13" s="50">
+        <v>-1.6553414</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="47" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="48">
+        <v>9</v>
+      </c>
+      <c r="E14" s="50">
+        <v>-1.9554927</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="47" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="48">
+        <v>7</v>
+      </c>
+      <c r="E15" s="50">
+        <v>-0.96700390000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="47" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="48">
+        <v>9</v>
+      </c>
+      <c r="E16" s="50">
+        <v>-0.58903890000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="47" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="48">
+        <v>4</v>
+      </c>
+      <c r="E17" s="50">
+        <v>-1.781598</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="47" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="48">
+        <v>9</v>
+      </c>
+      <c r="E18" s="50">
+        <v>-0.76994030000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="47" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="48">
+        <v>5</v>
+      </c>
+      <c r="E19" s="50">
+        <v>-0.5446124</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="47" t="s">
+        <v>18</v>
+      </c>
+      <c r="D20" s="48">
+        <v>7</v>
+      </c>
+      <c r="E20" s="50">
+        <v>-0.99867790000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="48">
+        <v>10</v>
+      </c>
+      <c r="E21" s="50">
+        <v>-1.2728577999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="47" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="48">
+        <v>5</v>
+      </c>
+      <c r="E22" s="50">
+        <v>-0.72989910000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="48">
+        <v>8</v>
+      </c>
+      <c r="E23" s="50">
+        <v>-1.4474084</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="48">
+        <v>8</v>
+      </c>
+      <c r="E24" s="50">
+        <v>-0.7162731</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B25" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="48">
+        <v>12</v>
+      </c>
+      <c r="E25" s="50">
+        <v>-1.4490105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="47" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="48">
+        <v>6</v>
+      </c>
+      <c r="E26" s="50">
+        <v>-1.4627169</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B27" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="47" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="48">
+        <v>5</v>
+      </c>
+      <c r="E27" s="50">
+        <v>-1.8195691000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B28" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D28" s="48">
+        <v>7</v>
+      </c>
+      <c r="E28" s="50">
+        <v>-0.93058200000000002</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B29" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="47" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="48">
+        <v>12</v>
+      </c>
+      <c r="E29" s="50">
+        <v>-1.7653719000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B30" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="47" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="48">
+        <v>11</v>
+      </c>
+      <c r="E30" s="50">
+        <v>-1.8356532999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="C31" s="47" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="48">
+        <v>7</v>
+      </c>
+      <c r="E31" s="50">
+        <v>-1.6925002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="47" t="s">
+        <v>31</v>
+      </c>
+      <c r="D32" s="48">
+        <v>13</v>
+      </c>
+      <c r="E32" s="50">
+        <v>-0.49685240000000003</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="47" t="s">
+        <v>32</v>
+      </c>
+      <c r="D33" s="48">
+        <v>11</v>
+      </c>
+      <c r="E33" s="50">
+        <v>-1.1239756999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="D34" s="48">
+        <v>9</v>
+      </c>
+      <c r="E34" s="50">
+        <v>-0.95115970000000005</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="D35" s="48">
+        <v>10</v>
+      </c>
+      <c r="E35" s="50">
+        <v>-1.1527605000000001</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C36" s="47" t="s">
+        <v>55</v>
+      </c>
+      <c r="D36" s="48">
+        <v>14</v>
+      </c>
+      <c r="E36" s="50">
+        <v>-1.9681147000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="D37" s="48">
+        <v>8</v>
+      </c>
+      <c r="E37" s="50">
+        <v>-1.4797013000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C38" s="47" t="s">
+        <v>57</v>
+      </c>
+      <c r="D38" s="48">
+        <v>15</v>
+      </c>
+      <c r="E38" s="50">
+        <v>-0.66219790000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C39" s="47" t="s">
+        <v>58</v>
+      </c>
+      <c r="D39" s="48">
+        <v>9</v>
+      </c>
+      <c r="E39" s="50">
+        <v>-1.0518787999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C40" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40" s="48">
+        <v>10</v>
+      </c>
+      <c r="E40" s="50">
+        <v>-2.1420286000000002</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B41" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="47" t="s">
+        <v>60</v>
+      </c>
+      <c r="D41" s="48">
+        <v>12</v>
+      </c>
+      <c r="E41" s="50">
+        <v>-1.558632</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C42" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="D42" s="48">
+        <v>8</v>
+      </c>
+      <c r="E42" s="50">
+        <v>-0.91209169999999995</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C43" s="47" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" s="48">
+        <v>13</v>
+      </c>
+      <c r="E43" s="50">
+        <v>-1.5218938</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" s="47" t="s">
+        <v>64</v>
+      </c>
+      <c r="D44" s="48">
+        <v>15</v>
+      </c>
+      <c r="E44" s="50">
+        <v>-2.3015219999999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="D45" s="48">
+        <v>13</v>
+      </c>
+      <c r="E45" s="50">
+        <v>-1.5561642</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C46" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="D46" s="48">
+        <v>12</v>
+      </c>
+      <c r="E46" s="50">
+        <v>-2.0662834000000001</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B47" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" s="47" t="s">
+        <v>67</v>
+      </c>
+      <c r="D47" s="48">
+        <v>10</v>
+      </c>
+      <c r="E47" s="50">
+        <v>-0.82010139999999998</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B48" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C48" s="47" t="s">
+        <v>68</v>
+      </c>
+      <c r="D48" s="48">
+        <v>7</v>
+      </c>
+      <c r="E48" s="50">
+        <v>-0.73003070000000003</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B49" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C49" s="47" t="s">
+        <v>69</v>
+      </c>
+      <c r="D49" s="48">
+        <v>12</v>
+      </c>
+      <c r="E49" s="50">
+        <v>-1.9224398</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B50" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C50" s="47" t="s">
+        <v>71</v>
+      </c>
+      <c r="D50" s="48">
+        <v>10</v>
+      </c>
+      <c r="E50" s="50">
+        <v>-1.7097344000000001</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B51" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C51" s="47" t="s">
+        <v>72</v>
+      </c>
+      <c r="D51" s="48">
+        <v>12</v>
+      </c>
+      <c r="E51" s="50">
+        <v>-1.1945570999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" s="47" t="s">
+        <v>73</v>
+      </c>
+      <c r="D52" s="48">
+        <v>8</v>
+      </c>
+      <c r="E52" s="50">
+        <v>-1.3800448999999999</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B53" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" s="47" t="s">
+        <v>74</v>
+      </c>
+      <c r="D53" s="48">
+        <v>15</v>
+      </c>
+      <c r="E53" s="50">
+        <v>-1.7164987</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B54" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C54" s="47" t="s">
+        <v>75</v>
+      </c>
+      <c r="D54" s="48">
+        <v>14</v>
+      </c>
+      <c r="E54" s="50">
+        <v>-0.39799400000000001</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B55" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="D55" s="48">
+        <v>15</v>
+      </c>
+      <c r="E55" s="50">
+        <v>-1.9292361</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B56" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C56" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="D56" s="48">
+        <v>15</v>
+      </c>
+      <c r="E56" s="50">
+        <v>-1.6710577</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B57" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C57" s="47" t="s">
+        <v>78</v>
+      </c>
+      <c r="D57" s="48">
+        <v>17</v>
+      </c>
+      <c r="E57" s="50">
+        <v>-1.6061728</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B58" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C58" s="47" t="s">
+        <v>44</v>
+      </c>
+      <c r="D58" s="48">
+        <v>10</v>
+      </c>
+      <c r="E58" s="50">
+        <v>-1.4736254</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B59" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C59" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="D59" s="48">
+        <v>13</v>
+      </c>
+      <c r="E59" s="50">
+        <v>-1.1503479000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B60" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C60" s="47" t="s">
+        <v>46</v>
+      </c>
+      <c r="D60" s="48">
+        <v>20</v>
+      </c>
+      <c r="E60" s="50">
+        <v>-2.0927213</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B61" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C61" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="D61" s="48">
+        <v>9</v>
+      </c>
+      <c r="E61" s="50">
+        <v>-0.55765520000000002</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B62" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C62" s="47" t="s">
+        <v>48</v>
+      </c>
+      <c r="D62" s="48">
+        <v>9</v>
+      </c>
+      <c r="E62" s="50">
+        <v>-0.86546460000000003</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B63" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C63" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="D63" s="48">
+        <v>12</v>
+      </c>
+      <c r="E63" s="50">
+        <v>-1.6195526</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B64" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C64" s="47" t="s">
+        <v>50</v>
+      </c>
+      <c r="D64" s="48">
+        <v>17</v>
+      </c>
+      <c r="E64" s="50">
+        <v>-2.0641634999999998</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B65" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C65" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="D65" s="48">
+        <v>9</v>
+      </c>
+      <c r="E65" s="50">
+        <v>-1.1969080000000001</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B66" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="C66" s="47" t="s">
+        <v>81</v>
+      </c>
+      <c r="D66" s="48">
+        <v>16</v>
+      </c>
+      <c r="E66" s="50">
+        <v>-1.2882861999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B67" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="C67" s="47" t="s">
+        <v>82</v>
+      </c>
+      <c r="D67" s="48">
+        <v>10</v>
+      </c>
+      <c r="E67" s="50">
+        <v>-0.60446739999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B68" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="C68" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="D68" s="48">
+        <v>14</v>
+      </c>
+      <c r="E68" s="50">
+        <v>-2.2311687</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B69" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="C69" s="47" t="s">
+        <v>84</v>
+      </c>
+      <c r="D69" s="48">
+        <v>13</v>
+      </c>
+      <c r="E69" s="50">
+        <v>-1.9450403000000001</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B70" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="C70" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="D70" s="48">
+        <v>11</v>
+      </c>
+      <c r="E70" s="50">
+        <v>-1.5569033000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B71" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="C71" s="47" t="s">
+        <v>86</v>
+      </c>
+      <c r="D71" s="48">
+        <v>14</v>
+      </c>
+      <c r="E71" s="50">
+        <v>-1.8000639000000001</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B72" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="C72" s="47" t="s">
+        <v>87</v>
+      </c>
+      <c r="D72" s="48">
+        <v>13</v>
+      </c>
+      <c r="E72" s="50">
+        <v>-2.133219</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B73" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="C73" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="D73" s="48">
+        <v>13</v>
+      </c>
+      <c r="E73" s="50">
+        <v>-1.1021977999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B74" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C74" s="47" t="s">
+        <v>90</v>
+      </c>
+      <c r="D74" s="48">
+        <v>9</v>
+      </c>
+      <c r="E74" s="50">
+        <v>-1.1955308</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B75" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C75" s="47" t="s">
+        <v>91</v>
+      </c>
+      <c r="D75" s="48">
+        <v>15</v>
+      </c>
+      <c r="E75" s="50">
+        <v>-0.40539150000000002</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B76" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C76" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="D76" s="48">
+        <v>17</v>
+      </c>
+      <c r="E76" s="50">
+        <v>-2.364277</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B77" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C77" s="47" t="s">
+        <v>93</v>
+      </c>
+      <c r="D77" s="48">
+        <v>13</v>
+      </c>
+      <c r="E77" s="50">
+        <v>-2.2254472999999999</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C78" s="47" t="s">
+        <v>94</v>
+      </c>
+      <c r="D78" s="48">
+        <v>12</v>
+      </c>
+      <c r="E78" s="50">
+        <v>-1.2299203999999999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B79" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C79" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="D79" s="48">
+        <v>23</v>
+      </c>
+      <c r="E79" s="50">
+        <v>-2.5229900000000001</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C80" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="D80" s="48">
+        <v>15</v>
+      </c>
+      <c r="E80" s="50">
+        <v>-1.8055378</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B81" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C81" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="D81" s="48">
+        <v>9</v>
+      </c>
+      <c r="E81" s="50">
+        <v>-0.17872080000000001</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B82" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="C82" s="47" t="s">
+        <v>99</v>
+      </c>
+      <c r="D82" s="48">
+        <v>6</v>
+      </c>
+      <c r="E82" s="50">
+        <v>-0.95027919999999999</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B83" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="C83" s="47" t="s">
+        <v>100</v>
+      </c>
+      <c r="D83" s="48">
+        <v>5</v>
+      </c>
+      <c r="E83" s="50">
+        <v>-0.35372510000000001</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A84" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B84" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="C84" s="47" t="s">
+        <v>101</v>
+      </c>
+      <c r="D84" s="48">
+        <v>10</v>
+      </c>
+      <c r="E84" s="50">
+        <v>-1.0465471</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A85" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B85" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="C85" s="47" t="s">
+        <v>102</v>
+      </c>
+      <c r="D85" s="48">
+        <v>5</v>
+      </c>
+      <c r="E85" s="50">
+        <v>-0.53988369999999997</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A86" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B86" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="C86" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="D86" s="48">
+        <v>5</v>
+      </c>
+      <c r="E86" s="50">
+        <v>-0.88302000000000003</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A87" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B87" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="C87" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="D87" s="48">
+        <v>7</v>
+      </c>
+      <c r="E87" s="50">
+        <v>-1.8016413</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B88" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="C88" s="47" t="s">
+        <v>105</v>
+      </c>
+      <c r="D88" s="48">
+        <v>8</v>
+      </c>
+      <c r="E88" s="50">
+        <v>-0.81582200000000005</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B89" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="C89" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="D89" s="48">
+        <v>4</v>
+      </c>
+      <c r="E89" s="50">
+        <v>-1.3434257999999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A90" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B90" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="C90" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="D90" s="48">
+        <v>5</v>
+      </c>
+      <c r="E90" s="50">
+        <v>-0.3823358</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B91" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="C91" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="D91" s="48">
+        <v>10</v>
+      </c>
+      <c r="E91" s="50">
+        <v>-0.37425829999999999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B92" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="C92" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="D92" s="48">
+        <v>11</v>
+      </c>
+      <c r="E92" s="50">
+        <v>-1.0823436</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B93" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="C93" s="47" t="s">
+        <v>111</v>
+      </c>
+      <c r="D93" s="48">
+        <v>15</v>
+      </c>
+      <c r="E93" s="50">
+        <v>-2.0292539999999999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B94" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="C94" s="47" t="s">
+        <v>112</v>
+      </c>
+      <c r="D94" s="48">
+        <v>14</v>
+      </c>
+      <c r="E94" s="50">
+        <v>-1.9568425</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B95" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="C95" s="47" t="s">
+        <v>113</v>
+      </c>
+      <c r="D95" s="48">
+        <v>21</v>
+      </c>
+      <c r="E95" s="50">
+        <v>-1.5870799</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B96" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="C96" s="47" t="s">
+        <v>114</v>
+      </c>
+      <c r="D96" s="48">
+        <v>16</v>
+      </c>
+      <c r="E96" s="50">
+        <v>-2.2375930999999998</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B97" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="C97" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="D97" s="48">
+        <v>9</v>
+      </c>
+      <c r="E97" s="50">
+        <v>-1.3065511000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22FE3B53-7B10-B94F-B8F7-BD145AC24ACE}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="15.5" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="46" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1" s="55" t="s">
+        <v>140</v>
+      </c>
+      <c r="E1" s="55" t="s">
+        <v>141</v>
+      </c>
+      <c r="F1" s="55" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="48">
+        <v>13</v>
+      </c>
+      <c r="D2" s="54">
+        <v>13</v>
+      </c>
+      <c r="E2" s="54">
+        <v>25</v>
+      </c>
+      <c r="F2" s="54">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="48">
+        <v>13</v>
+      </c>
+      <c r="D3" s="54">
+        <v>9</v>
+      </c>
+      <c r="E3" s="54">
+        <v>25</v>
+      </c>
+      <c r="F3" s="54">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="48">
+        <v>8</v>
+      </c>
+      <c r="D4" s="54">
+        <v>7</v>
+      </c>
+      <c r="E4" s="54">
+        <v>21</v>
+      </c>
+      <c r="F4" s="54">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="47" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="48">
+        <v>11</v>
+      </c>
+      <c r="D5" s="54">
+        <v>10</v>
+      </c>
+      <c r="E5" s="54">
+        <v>25</v>
+      </c>
+      <c r="F5" s="54">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="48">
+        <v>11</v>
+      </c>
+      <c r="D6" s="54">
+        <v>10</v>
+      </c>
+      <c r="E6" s="54">
+        <v>30</v>
+      </c>
+      <c r="F6" s="54">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="48">
+        <v>17</v>
+      </c>
+      <c r="D7" s="54">
+        <v>15</v>
+      </c>
+      <c r="E7" s="54">
+        <v>29</v>
+      </c>
+      <c r="F7" s="54">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A8" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="48">
+        <v>13</v>
+      </c>
+      <c r="D8" s="54">
+        <v>16</v>
+      </c>
+      <c r="E8" s="54">
+        <v>34</v>
+      </c>
+      <c r="F8" s="54">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A9" s="47" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="47" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="48">
+        <v>17</v>
+      </c>
+      <c r="D9" s="54">
+        <v>20</v>
+      </c>
+      <c r="E9" s="54">
+        <v>40</v>
+      </c>
+      <c r="F9" s="54">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="48">
+        <v>13</v>
+      </c>
+      <c r="D10" s="54">
+        <v>16</v>
+      </c>
+      <c r="E10" s="54">
+        <v>39</v>
+      </c>
+      <c r="F10" s="54">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="47" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="48">
+        <v>13</v>
+      </c>
+      <c r="D11" s="54">
+        <v>17</v>
+      </c>
+      <c r="E11" s="54">
+        <v>42</v>
+      </c>
+      <c r="F11" s="54">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="48">
+        <v>9</v>
+      </c>
+      <c r="D12" s="54">
+        <v>8</v>
+      </c>
+      <c r="E12" s="54">
+        <v>24</v>
+      </c>
+      <c r="F12" s="54">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="48">
+        <v>18</v>
+      </c>
+      <c r="D13" s="54">
+        <v>17</v>
+      </c>
+      <c r="E13" s="54">
+        <v>44</v>
+      </c>
+      <c r="F13" s="54">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1BBFA41-B47D-3845-8ACD-871870FF0964}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="51" t="s">
+        <v>116</v>
+      </c>
+      <c r="D1" s="51" t="s">
+        <v>139</v>
+      </c>
+      <c r="E1" s="51" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" s="53">
+        <v>-1.851592931351506</v>
+      </c>
+      <c r="E2" s="53">
+        <v>-1.9787381347650597</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="52" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="52" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="53">
+        <v>-1.6560822841844116</v>
+      </c>
+      <c r="E3" s="53">
+        <v>-1.9244274826174834</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="52" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="52" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="53">
+        <v>-1.250226828509698</v>
+      </c>
+      <c r="E4" s="53">
+        <v>-1.5274967242746265</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="52" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="D5" s="53">
+        <v>-1.2715936618544514</v>
+      </c>
+      <c r="E5" s="53">
+        <v>-1.452128160523952</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A6" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="52" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="53">
+        <v>-1.5804635240431175</v>
+      </c>
+      <c r="E6" s="53">
+        <v>-1.7316792067768285</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="53">
+        <v>-1.5965149563286907</v>
+      </c>
+      <c r="E7" s="53">
+        <v>-1.8159780865259094</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A8" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="52" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="53">
+        <v>-2.1409557346098875</v>
+      </c>
+      <c r="E8" s="53">
+        <v>-2.3809542406896171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="48" x14ac:dyDescent="0.2">
+      <c r="A9" s="52" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" s="53">
+        <v>-1.9406669766607496</v>
+      </c>
+      <c r="E9" s="53">
+        <v>-2.5009381832037509</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A10" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="C10" s="52" t="s">
+        <v>125</v>
+      </c>
+      <c r="D10" s="53">
+        <v>-2.2013467629332113</v>
+      </c>
+      <c r="E10" s="53">
+        <v>-2.5422511749436167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="52" t="s">
+        <v>126</v>
+      </c>
+      <c r="D11" s="53">
+        <v>-1.277045634911196</v>
+      </c>
+      <c r="E11" s="53">
+        <v>-1.9802140586191881</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="B12" s="52" t="s">
+        <v>98</v>
+      </c>
+      <c r="C12" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="D12" s="53">
+        <v>-1.1000064436416255</v>
+      </c>
+      <c r="E12" s="53">
+        <v>-1.3142218460755688</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A13" s="52" t="s">
+        <v>79</v>
+      </c>
+      <c r="B13" s="52" t="s">
+        <v>107</v>
+      </c>
+      <c r="C13" s="52" t="s">
+        <v>128</v>
+      </c>
+      <c r="D13" s="53">
+        <v>-2.8038026433619021</v>
+      </c>
+      <c r="E13" s="53">
+        <v>-2.6819737972522342</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>